<commit_message>
Update data source document
</commit_message>
<xml_diff>
--- a/docs/info/Data Source.xlsx
+++ b/docs/info/Data Source.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27715"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andersonfrailey/taxdata/docs/info/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="0" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
+    <workbookView xWindow="8740" yWindow="460" windowWidth="16540" windowHeight="14320" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Stage I growth rate source" sheetId="1" r:id="rId1"/>
@@ -12,6 +17,9 @@
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -55,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="166">
   <si>
     <t>Target</t>
   </si>
@@ -498,6 +506,63 @@
   </si>
   <si>
     <t>Census</t>
+  </si>
+  <si>
+    <t>CPI Medicare</t>
+  </si>
+  <si>
+    <t>Table 2.3</t>
+  </si>
+  <si>
+    <t>Supplemental Income: Net Income Amount</t>
+  </si>
+  <si>
+    <t>Supplemental Income: Net Loss Amount</t>
+  </si>
+  <si>
+    <t>Column 66</t>
+  </si>
+  <si>
+    <t>Columns 14 + 27 + 53</t>
+  </si>
+  <si>
+    <t>Column 40</t>
+  </si>
+  <si>
+    <t>Column 69</t>
+  </si>
+  <si>
+    <t>Column 6</t>
+  </si>
+  <si>
+    <t>Column 8</t>
+  </si>
+  <si>
+    <t>Column 12</t>
+  </si>
+  <si>
+    <t>Column 20</t>
+  </si>
+  <si>
+    <t>Column 22</t>
+  </si>
+  <si>
+    <t>Column 26</t>
+  </si>
+  <si>
+    <t>Column 38</t>
+  </si>
+  <si>
+    <t>Columns 52 + 56 + 60</t>
+  </si>
+  <si>
+    <t>Columns 54 + 58 + 62</t>
+  </si>
+  <si>
+    <t>Column 70</t>
+  </si>
+  <si>
+    <t>Column 68</t>
   </si>
 </sst>
 </file>
@@ -633,6 +698,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -960,11 +1030,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="42.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="42.6640625" customWidth="1"/>
@@ -972,7 +1042,7 @@
     <col min="5" max="5" width="43" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>79</v>
       </c>
@@ -990,7 +1060,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1010,7 +1080,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1030,7 +1100,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1050,7 +1120,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1070,7 +1140,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1090,7 +1160,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1110,7 +1180,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1130,7 +1200,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1147,7 +1217,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1161,7 +1231,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1181,7 +1251,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1198,7 +1268,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1218,7 +1288,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1235,7 +1305,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="30">
+    <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1255,7 +1325,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1275,7 +1345,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1285,11 +1355,14 @@
       <c r="C17" t="s">
         <v>116</v>
       </c>
+      <c r="E17" t="s">
+        <v>147</v>
+      </c>
       <c r="F17" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1316,31 +1389,26 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="42.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="42.33203125" customWidth="1"/>
-    <col min="5" max="5" width="36.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>79</v>
       </c>
@@ -1354,14 +1422,15 @@
         <v>1</v>
       </c>
       <c r="E1" s="7"/>
-      <c r="F1" t="s">
+      <c r="F1" s="7"/>
+      <c r="G1" t="s">
         <v>95</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -1372,8 +1441,9 @@
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="G2" s="6"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1383,14 +1453,14 @@
       <c r="D3" t="s">
         <v>81</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>52</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1404,13 +1474,16 @@
         <v>81</v>
       </c>
       <c r="E4" t="s">
+        <v>151</v>
+      </c>
+      <c r="F4" t="s">
         <v>82</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1424,13 +1497,16 @@
         <v>81</v>
       </c>
       <c r="E5" t="s">
+        <v>152</v>
+      </c>
+      <c r="F5" t="s">
         <v>144</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1444,13 +1520,16 @@
         <v>81</v>
       </c>
       <c r="E6" t="s">
+        <v>153</v>
+      </c>
+      <c r="F6" t="s">
         <v>83</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1464,13 +1543,16 @@
         <v>80</v>
       </c>
       <c r="E7" t="s">
+        <v>154</v>
+      </c>
+      <c r="F7" t="s">
         <v>87</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1480,11 +1562,20 @@
       <c r="C8" t="s">
         <v>122</v>
       </c>
+      <c r="D8" t="s">
+        <v>148</v>
+      </c>
+      <c r="E8" t="s">
+        <v>155</v>
+      </c>
       <c r="F8" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1498,13 +1589,16 @@
         <v>80</v>
       </c>
       <c r="E9" t="s">
+        <v>156</v>
+      </c>
+      <c r="F9" t="s">
         <v>88</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1518,13 +1612,16 @@
         <v>80</v>
       </c>
       <c r="E10" t="s">
+        <v>157</v>
+      </c>
+      <c r="F10" t="s">
         <v>92</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1538,13 +1635,16 @@
         <v>80</v>
       </c>
       <c r="E11" t="s">
+        <v>158</v>
+      </c>
+      <c r="F11" t="s">
         <v>89</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1558,13 +1658,16 @@
         <v>80</v>
       </c>
       <c r="E12" t="s">
+        <v>159</v>
+      </c>
+      <c r="F12" t="s">
         <v>90</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1578,13 +1681,16 @@
         <v>93</v>
       </c>
       <c r="E13" t="s">
+        <v>160</v>
+      </c>
+      <c r="F13" t="s">
         <v>94</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1598,13 +1704,16 @@
         <v>80</v>
       </c>
       <c r="E14" t="s">
+        <v>161</v>
+      </c>
+      <c r="F14" t="s">
         <v>91</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1614,11 +1723,20 @@
       <c r="C15" t="s">
         <v>126</v>
       </c>
+      <c r="D15" t="s">
+        <v>80</v>
+      </c>
+      <c r="E15" t="s">
+        <v>162</v>
+      </c>
       <c r="F15" t="s">
+        <v>149</v>
+      </c>
+      <c r="G15" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1628,11 +1746,20 @@
       <c r="C16" t="s">
         <v>127</v>
       </c>
+      <c r="D16" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" t="s">
+        <v>163</v>
+      </c>
       <c r="F16" t="s">
+        <v>150</v>
+      </c>
+      <c r="G16" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1646,13 +1773,16 @@
         <v>80</v>
       </c>
       <c r="E17" t="s">
+        <v>164</v>
+      </c>
+      <c r="F17" t="s">
         <v>86</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1666,13 +1796,16 @@
         <v>80</v>
       </c>
       <c r="E18" t="s">
+        <v>165</v>
+      </c>
+      <c r="F18" t="s">
         <v>85</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1686,13 +1819,16 @@
         <v>80</v>
       </c>
       <c r="E19" t="s">
+        <v>155</v>
+      </c>
+      <c r="F19" t="s">
         <v>84</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1706,13 +1842,16 @@
         <v>80</v>
       </c>
       <c r="E20" t="s">
+        <v>155</v>
+      </c>
+      <c r="F20" t="s">
         <v>84</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1726,13 +1865,16 @@
         <v>80</v>
       </c>
       <c r="E21" t="s">
+        <v>155</v>
+      </c>
+      <c r="F21" t="s">
         <v>84</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1746,13 +1888,16 @@
         <v>80</v>
       </c>
       <c r="E22" t="s">
+        <v>155</v>
+      </c>
+      <c r="F22" t="s">
         <v>84</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1766,13 +1911,16 @@
         <v>80</v>
       </c>
       <c r="E23" t="s">
+        <v>155</v>
+      </c>
+      <c r="F23" t="s">
         <v>84</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1786,13 +1934,16 @@
         <v>80</v>
       </c>
       <c r="E24" t="s">
+        <v>155</v>
+      </c>
+      <c r="F24" t="s">
         <v>84</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1806,13 +1957,16 @@
         <v>80</v>
       </c>
       <c r="E25" t="s">
+        <v>155</v>
+      </c>
+      <c r="F25" t="s">
         <v>84</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1826,13 +1980,16 @@
         <v>80</v>
       </c>
       <c r="E26" t="s">
+        <v>155</v>
+      </c>
+      <c r="F26" t="s">
         <v>84</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1846,13 +2003,16 @@
         <v>80</v>
       </c>
       <c r="E27" t="s">
+        <v>155</v>
+      </c>
+      <c r="F27" t="s">
         <v>84</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1866,13 +2026,16 @@
         <v>80</v>
       </c>
       <c r="E28" t="s">
+        <v>155</v>
+      </c>
+      <c r="F28" t="s">
         <v>84</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1886,13 +2049,16 @@
         <v>80</v>
       </c>
       <c r="E29" t="s">
+        <v>155</v>
+      </c>
+      <c r="F29" t="s">
         <v>84</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1906,22 +2072,20 @@
         <v>80</v>
       </c>
       <c r="E30" t="s">
+        <v>155</v>
+      </c>
+      <c r="F30" t="s">
         <v>84</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>37</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D1:F1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>